<commit_message>
Excel File Read Completed
</commit_message>
<xml_diff>
--- a/TestData/User_Dashboard.xlsx
+++ b/TestData/User_Dashboard.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10712370\PycharmProjects\pythonProject\BPxPoc\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D90E99-EE44-42AC-92B6-77FAD7119BC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCE42A50-EA85-4382-9B49-620809AC8D9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Portal" sheetId="1" r:id="rId1"/>
     <sheet name="OneMapRouting" sheetId="2" r:id="rId2"/>
+    <sheet name="Arc_GIS" sheetId="3" r:id="rId3"/>
+    <sheet name="Master" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="100">
   <si>
     <t>LAVERNE 58-T2-12X1 3B B302H</t>
   </si>
@@ -80,13 +82,259 @@
   </si>
   <si>
     <t>GPS_Source_Input</t>
+  </si>
+  <si>
+    <t>Business_Unit_Input</t>
+  </si>
+  <si>
+    <t>Facility_Input</t>
+  </si>
+  <si>
+    <t>Gateway_Input</t>
+  </si>
+  <si>
+    <t>Permian</t>
+  </si>
+  <si>
+    <t>GRAND SLAM CDP</t>
+  </si>
+  <si>
+    <t>ngw-perm-ms-001</t>
+  </si>
+  <si>
+    <t>ArcGIS_Business_Unit_DD</t>
+  </si>
+  <si>
+    <t>ArcGIS_Facility_DD</t>
+  </si>
+  <si>
+    <t>ArcGIS_Gateway_DD</t>
+  </si>
+  <si>
+    <t>ArcGIS_Device_DD</t>
+  </si>
+  <si>
+    <t>Eagle Ford Black Hawk</t>
+  </si>
+  <si>
+    <t>Eagle Ford Hawkville</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>BINGO CDP</t>
+  </si>
+  <si>
+    <t>BISHOP SWD</t>
+  </si>
+  <si>
+    <t>BLACKHAWK CENTRAL CDP</t>
+  </si>
+  <si>
+    <t>BLACKHAWK NORTHEAST CDP</t>
+  </si>
+  <si>
+    <t>BLACKHAWK SOUTHWEST CDP</t>
+  </si>
+  <si>
+    <t>CHECKMATE CDP</t>
+  </si>
+  <si>
+    <t>HAWKVILLE CENTRAL CDP</t>
+  </si>
+  <si>
+    <t>HAWKVILLE FAR EAST CDP</t>
+  </si>
+  <si>
+    <t>HAWKVILLE NORTHEAST CDP</t>
+  </si>
+  <si>
+    <t>KARNES CDP</t>
+  </si>
+  <si>
+    <t>WATERFALL 56-T2-15 FACILITY PAD</t>
+  </si>
+  <si>
+    <t>Device_Input</t>
+  </si>
+  <si>
+    <t>ngw-ef-ms-001</t>
+  </si>
+  <si>
+    <t>ngw-ef-ms-002</t>
+  </si>
+  <si>
+    <t>ngw-ef-ms-003</t>
+  </si>
+  <si>
+    <t>ngw-ef-ms-004</t>
+  </si>
+  <si>
+    <t>ngw-ef-ms-005</t>
+  </si>
+  <si>
+    <t>ngw-ef-ms-007</t>
+  </si>
+  <si>
+    <t>ngw-ef-ms-011</t>
+  </si>
+  <si>
+    <t>ngw-ef-ms-012</t>
+  </si>
+  <si>
+    <t>ngw-ef-ms-013</t>
+  </si>
+  <si>
+    <t>ngw-ef-ms-014</t>
+  </si>
+  <si>
+    <t>ngw-ef-ms-015</t>
+  </si>
+  <si>
+    <t>ngw-ef-ms-016</t>
+  </si>
+  <si>
+    <t>ngw-ef-ms-017</t>
+  </si>
+  <si>
+    <t>ngw-ef-ms-018</t>
+  </si>
+  <si>
+    <t>ngw-ef-ms-019</t>
+  </si>
+  <si>
+    <t>ngw-ef-ms-020</t>
+  </si>
+  <si>
+    <t>ngw-ef-ms-021</t>
+  </si>
+  <si>
+    <t>ngw-ef-ms-022</t>
+  </si>
+  <si>
+    <t>ngw-ef-ms-023</t>
+  </si>
+  <si>
+    <t>ngw-ef-ms-024</t>
+  </si>
+  <si>
+    <t>ngw-ef-ms-025</t>
+  </si>
+  <si>
+    <t>ngw-ef-ms-026</t>
+  </si>
+  <si>
+    <t>ngw-ef-ms-027</t>
+  </si>
+  <si>
+    <t>ngw-ef-ms-028</t>
+  </si>
+  <si>
+    <t>ngw-ef-ms-029</t>
+  </si>
+  <si>
+    <t>ngw-ef-ms-031</t>
+  </si>
+  <si>
+    <t>ngw-ef-ms-032</t>
+  </si>
+  <si>
+    <t>ngw-ef-ms-033</t>
+  </si>
+  <si>
+    <t>ngw-ef-ms-034</t>
+  </si>
+  <si>
+    <t>ngw-perm-ms-002</t>
+  </si>
+  <si>
+    <t>ngw-perm-ms-003</t>
+  </si>
+  <si>
+    <t>ngw-perm-ms-004</t>
+  </si>
+  <si>
+    <t>ngw-perm-ms-005</t>
+  </si>
+  <si>
+    <t>ngw-perm-ms-006</t>
+  </si>
+  <si>
+    <t>ngw-perm-ms-008</t>
+  </si>
+  <si>
+    <t>ngw-perm-ms-009</t>
+  </si>
+  <si>
+    <t>ngw-perm-ms-010</t>
+  </si>
+  <si>
+    <t>ngw-perm-ms-011</t>
+  </si>
+  <si>
+    <t>ngw-perm-ms-012</t>
+  </si>
+  <si>
+    <t>ngw-perm-ms-013</t>
+  </si>
+  <si>
+    <t>ngw-perm-ms-014</t>
+  </si>
+  <si>
+    <t>ngw-perm-ms-15</t>
+  </si>
+  <si>
+    <t>ngw-perm-ms-16</t>
+  </si>
+  <si>
+    <t>ngw-perm-ms-17</t>
+  </si>
+  <si>
+    <t>ngw-perm-ms-18</t>
+  </si>
+  <si>
+    <t>ngw-perm-ms-19</t>
+  </si>
+  <si>
+    <t>ngw-perm-ms-20</t>
+  </si>
+  <si>
+    <t>mn-m10</t>
+  </si>
+  <si>
+    <t>nm-gw01</t>
+  </si>
+  <si>
+    <t>nm-m01</t>
+  </si>
+  <si>
+    <t>nm-m02</t>
+  </si>
+  <si>
+    <t>nm-m03</t>
+  </si>
+  <si>
+    <t>nm-m04</t>
+  </si>
+  <si>
+    <t>nm-m05</t>
+  </si>
+  <si>
+    <t>nm-m06</t>
+  </si>
+  <si>
+    <t>nm-m07</t>
+  </si>
+  <si>
+    <t>nm-m08</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,6 +388,18 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -189,7 +449,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -217,6 +477,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -560,8 +821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEBDEB91-7A76-4256-939D-7307DD95B04D}">
   <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="24.95" customHeight="1"/>
@@ -791,4 +1052,640 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D2E5C8E-15B7-4737-BC2D-FBAA4C5B451D}">
+  <dimension ref="A1:B45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="24.95" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="26.42578125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="104.85546875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="10" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="9" customFormat="1" ht="24.95" customHeight="1">
+      <c r="A1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="24.95" customHeight="1">
+      <c r="A2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="24.95" customHeight="1">
+      <c r="A3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="24.95" customHeight="1">
+      <c r="A4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="24.95" customHeight="1">
+      <c r="A5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="24.95" customHeight="1">
+      <c r="A6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="24.95" customHeight="1">
+      <c r="A7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="24.95" customHeight="1">
+      <c r="A8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="24.95" customHeight="1">
+      <c r="A9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="24.95" customHeight="1">
+      <c r="A10" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="3"/>
+    </row>
+    <row r="11" spans="1:2" ht="24.95" customHeight="1">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+    </row>
+    <row r="12" spans="1:2" ht="24.95" customHeight="1">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+    </row>
+    <row r="13" spans="1:2" ht="24.95" customHeight="1">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+    </row>
+    <row r="14" spans="1:2" ht="24.95" customHeight="1">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+    </row>
+    <row r="15" spans="1:2" ht="24.95" customHeight="1">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+    </row>
+    <row r="16" spans="1:2" ht="24.95" customHeight="1">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+    </row>
+    <row r="17" spans="1:2" ht="24.95" customHeight="1">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+    </row>
+    <row r="18" spans="1:2" ht="24.95" customHeight="1">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+    </row>
+    <row r="19" spans="1:2" ht="24.95" customHeight="1">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+    </row>
+    <row r="20" spans="1:2" ht="24.95" customHeight="1">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+    </row>
+    <row r="21" spans="1:2" ht="24.95" customHeight="1">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+    </row>
+    <row r="22" spans="1:2" ht="24.95" customHeight="1">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+    </row>
+    <row r="23" spans="1:2" ht="24.95" customHeight="1">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+    </row>
+    <row r="24" spans="1:2" ht="24.95" customHeight="1">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+    </row>
+    <row r="25" spans="1:2" ht="24.95" customHeight="1">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+    </row>
+    <row r="26" spans="1:2" ht="24.95" customHeight="1">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+    </row>
+    <row r="27" spans="1:2" ht="24.95" customHeight="1">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+    </row>
+    <row r="28" spans="1:2" ht="24.95" customHeight="1">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+    </row>
+    <row r="29" spans="1:2" ht="24.95" customHeight="1">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+    </row>
+    <row r="30" spans="1:2" ht="24.95" customHeight="1">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+    </row>
+    <row r="31" spans="1:2" ht="24.95" customHeight="1">
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+    </row>
+    <row r="32" spans="1:2" ht="24.95" customHeight="1">
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
+    </row>
+    <row r="33" spans="1:2" ht="24.95" customHeight="1">
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
+    </row>
+    <row r="34" spans="1:2" ht="24.95" customHeight="1">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+    </row>
+    <row r="35" spans="1:2" ht="24.95" customHeight="1">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+    </row>
+    <row r="36" spans="1:2" ht="24.95" customHeight="1">
+      <c r="A36" s="3"/>
+      <c r="B36" s="3"/>
+    </row>
+    <row r="37" spans="1:2" ht="24.95" customHeight="1">
+      <c r="A37" s="3"/>
+      <c r="B37" s="3"/>
+    </row>
+    <row r="38" spans="1:2" ht="24.95" customHeight="1">
+      <c r="A38" s="3"/>
+      <c r="B38" s="3"/>
+    </row>
+    <row r="39" spans="1:2" ht="24.95" customHeight="1">
+      <c r="A39" s="3"/>
+      <c r="B39" s="3"/>
+    </row>
+    <row r="40" spans="1:2" ht="24.95" customHeight="1">
+      <c r="A40" s="3"/>
+      <c r="B40" s="3"/>
+    </row>
+    <row r="41" spans="1:2" ht="24.95" customHeight="1">
+      <c r="A41" s="3"/>
+      <c r="B41" s="3"/>
+    </row>
+    <row r="42" spans="1:2" ht="24.95" customHeight="1">
+      <c r="A42" s="3"/>
+      <c r="B42" s="3"/>
+    </row>
+    <row r="43" spans="1:2" ht="24.95" customHeight="1">
+      <c r="A43" s="3"/>
+      <c r="B43" s="3"/>
+    </row>
+    <row r="44" spans="1:2" ht="24.95" customHeight="1">
+      <c r="A44" s="3"/>
+      <c r="B44" s="3"/>
+    </row>
+    <row r="45" spans="1:2" ht="24.95" customHeight="1">
+      <c r="A45" s="3"/>
+      <c r="B45" s="3"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{7BC6D89C-D18A-47A1-905F-BD1A4D59672C}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{95CF9EC8-2DC8-4C0C-A0C9-4CE6A723F6DF}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{111973C2-9D97-4A4B-AFB4-802EECCDE59A}">
+          <x14:formula1>
+            <xm:f>Master!$A$2:$A$50</xm:f>
+          </x14:formula1>
+          <xm:sqref>B7</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{086EC8E2-0AD6-4493-A2F0-59987A987992}">
+          <x14:formula1>
+            <xm:f>Master!$B$2:$B$50</xm:f>
+          </x14:formula1>
+          <xm:sqref>B8</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{242D22E4-DC81-40A7-9D09-90AFBFEC5E6D}">
+          <x14:formula1>
+            <xm:f>Master!$C$2:$C$51</xm:f>
+          </x14:formula1>
+          <xm:sqref>B9</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F9DDDF2C-8797-43AA-8BF5-A191B673D3B0}">
+          <x14:formula1>
+            <xm:f>Master!$D$2:$D$44</xm:f>
+          </x14:formula1>
+          <xm:sqref>B10</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{359F2626-80DD-46FD-8FFC-A99C16C879FD}">
+  <dimension ref="A1:D50"/>
+  <sheetViews>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="31.7109375" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="B5" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="B6" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="B7" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="B8" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="B9" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="B10" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="B11" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="B12" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="B13" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="B14" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="C15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="C16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3">
+      <c r="C17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3">
+      <c r="C18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3">
+      <c r="C19" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3">
+      <c r="C20" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="3:3">
+      <c r="C21" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="3:3">
+      <c r="C22" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="3:3">
+      <c r="C23" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="3:3">
+      <c r="C24" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="3:3">
+      <c r="C25" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="3:3">
+      <c r="C26" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="3:3">
+      <c r="C27" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" spans="3:3">
+      <c r="C28" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="3:3">
+      <c r="C29" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="3:3">
+      <c r="C30" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="3:3">
+      <c r="C31" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="32" spans="3:3">
+      <c r="C32" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3">
+      <c r="C33" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" spans="3:3">
+      <c r="C34" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="3:3">
+      <c r="C35" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="36" spans="3:3">
+      <c r="C36" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="37" spans="3:3">
+      <c r="C37" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="38" spans="3:3">
+      <c r="C38" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="39" spans="3:3">
+      <c r="C39" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="40" spans="3:3">
+      <c r="C40" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" spans="3:3">
+      <c r="C41" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="42" spans="3:3">
+      <c r="C42" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="43" spans="3:3">
+      <c r="C43" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="44" spans="3:3">
+      <c r="C44" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="45" spans="3:3">
+      <c r="C45" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="46" spans="3:3">
+      <c r="C46" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="47" spans="3:3">
+      <c r="C47" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="48" spans="3:3">
+      <c r="C48" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="49" spans="3:3">
+      <c r="C49" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="50" spans="3:3">
+      <c r="C50" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="9" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>